<commit_message>
Updated itemized receipts spreadsheet and added new order invoices
</commit_message>
<xml_diff>
--- a/Ordered Parts/Itemized Receipts.xlsx
+++ b/Ordered Parts/Itemized Receipts.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="40">
   <si>
     <t>Description</t>
   </si>
@@ -36,12 +36,6 @@
     <t>Date of Purchase</t>
   </si>
   <si>
-    <t>Amazon Order</t>
-  </si>
-  <si>
-    <t>Amazon Order.pdf</t>
-  </si>
-  <si>
     <t>MPU-9250 Sensor, MPU-6050 Sensor, Jumper Wires, 3pc Arduino Nanos</t>
   </si>
   <si>
@@ -51,15 +45,9 @@
     <t>Brian</t>
   </si>
   <si>
-    <t>Hobby King Order</t>
-  </si>
-  <si>
     <t>Amazon Order 2</t>
   </si>
   <si>
-    <t>Hobby King Order.pdf</t>
-  </si>
-  <si>
     <t>Amazon Order 2.pdf</t>
   </si>
   <si>
@@ -100,6 +88,57 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>Amazon Order 5</t>
+  </si>
+  <si>
+    <t>Soldering Materials, Crimping tool, Silicone Wire, Alligator Clips, Heat Shrink Tubing, Resistors, Capacitors</t>
+  </si>
+  <si>
+    <t>Amazon Order 5.pdf</t>
+  </si>
+  <si>
+    <t>Amazon Order 1.pdf</t>
+  </si>
+  <si>
+    <t>Digi-Key Order</t>
+  </si>
+  <si>
+    <t>Digi-Key Order.pdf</t>
+  </si>
+  <si>
+    <t>Solder Wick, 0.1" Connectors (Male and Female), Crimp Contacts</t>
+  </si>
+  <si>
+    <t>Amazon Order 1</t>
+  </si>
+  <si>
+    <t>Hobby King Order 1</t>
+  </si>
+  <si>
+    <t>Hobby King Order 1.pdf</t>
+  </si>
+  <si>
+    <t>Arrow Order</t>
+  </si>
+  <si>
+    <t>Arrow Order.pdf</t>
+  </si>
+  <si>
+    <t>Slip Rings, Power MOSFETs, Rocker Switches</t>
+  </si>
+  <si>
+    <t>Amazon Order 6.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Soldering Station, Tip Cleaner, Tip Tinner, Extra Iron Tips </t>
+  </si>
+  <si>
+    <t>Amazon Order 6*</t>
+  </si>
+  <si>
+    <t>*Not sure if Feron will fund this order</t>
   </si>
 </sst>
 </file>
@@ -446,10 +485,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -470,7 +509,7 @@
         <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
@@ -484,131 +523,216 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="B2" s="5">
         <v>43032</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="E2" s="6">
         <v>35.65</v>
       </c>
       <c r="F2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="B3" s="5">
         <v>43033</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="E3" s="6">
         <v>48.12</v>
       </c>
       <c r="F3" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B4" s="5">
         <v>43033</v>
       </c>
       <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>9</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>13</v>
       </c>
       <c r="E4" s="6">
         <v>7.9</v>
       </c>
       <c r="F4" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B5" s="5">
         <v>43041</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="E5" s="6">
         <v>6.99</v>
       </c>
       <c r="F5" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B6" s="5">
         <v>43041</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E6" s="6">
         <v>13.99</v>
       </c>
       <c r="F6" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B7" s="5">
         <v>43045</v>
       </c>
       <c r="C7" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="E7" s="6">
         <v>87.13</v>
       </c>
       <c r="F7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="5">
+        <v>43084</v>
+      </c>
+      <c r="C8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>25</v>
       </c>
+      <c r="E8" s="6">
+        <v>149.87</v>
+      </c>
+      <c r="F8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="5">
+        <v>43084</v>
+      </c>
+      <c r="C9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" s="6">
+        <v>45.31</v>
+      </c>
+      <c r="F9" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="D10" s="1" t="s">
-        <v>26</v>
+      <c r="A10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" s="5">
+        <v>43084</v>
+      </c>
+      <c r="C10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>34</v>
       </c>
       <c r="E10" s="6">
-        <f>SUM(E2:E7)</f>
-        <v>199.77999999999997</v>
+        <v>45.22</v>
+      </c>
+      <c r="F10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" s="5">
+        <v>43084</v>
+      </c>
+      <c r="C11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E11" s="6">
+        <v>147.68</v>
+      </c>
+      <c r="F11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="D13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13" s="6">
+        <f>SUM(E2:E12)</f>
+        <v>587.8599999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -619,8 +743,12 @@
     <hyperlink ref="D5" r:id="rId4" xr:uid="{CDF8F3EF-15A0-4C77-B9A6-1524FB766AB3}"/>
     <hyperlink ref="D6" r:id="rId5" xr:uid="{4CED5BFD-DE36-479D-B4BF-86D4506AD48F}"/>
     <hyperlink ref="D7" r:id="rId6" xr:uid="{67ECE9F8-194A-4F00-8B7B-8270BD726FA7}"/>
+    <hyperlink ref="D8" r:id="rId7" xr:uid="{AEB29289-D001-4D0C-94B1-E43D7F0C5680}"/>
+    <hyperlink ref="D9" r:id="rId8" xr:uid="{8125CA67-8455-4019-B4E5-300A48922E7B}"/>
+    <hyperlink ref="D10" r:id="rId9" xr:uid="{F602FE1D-63A3-4465-AC92-51C421A80D61}"/>
+    <hyperlink ref="D11" r:id="rId10" xr:uid="{A4EDEC9A-1F76-44F4-9AC5-21D8B162BC12}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId7"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId11"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated part orders spreadsheet and invoices
</commit_message>
<xml_diff>
--- a/Ordered Parts/Itemized Receipts.xlsx
+++ b/Ordered Parts/Itemized Receipts.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18625"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18730"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -488,7 +488,7 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -675,7 +675,7 @@
         <v>28</v>
       </c>
       <c r="E9" s="6">
-        <v>45.31</v>
+        <v>52.58</v>
       </c>
       <c r="F9" t="s">
         <v>29</v>
@@ -727,7 +727,7 @@
       </c>
       <c r="E13" s="6">
         <f>SUM(E2:E12)</f>
-        <v>587.8599999999999</v>
+        <v>595.12999999999988</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">

</xml_diff>

<commit_message>
Added new Hobby King and Banggood Orders to itemized receipts sheet
</commit_message>
<xml_diff>
--- a/Ordered Parts/Itemized Receipts.xlsx
+++ b/Ordered Parts/Itemized Receipts.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="48">
   <si>
     <t>Description</t>
   </si>
@@ -102,12 +102,6 @@
     <t>Amazon Order 1.pdf</t>
   </si>
   <si>
-    <t>Digi-Key Order</t>
-  </si>
-  <si>
-    <t>Digi-Key Order.pdf</t>
-  </si>
-  <si>
     <t>Solder Wick, 0.1" Connectors (Male and Female), Crimp Contacts</t>
   </si>
   <si>
@@ -139,6 +133,36 @@
   </si>
   <si>
     <t>*Not sure if Feron will fund this order</t>
+  </si>
+  <si>
+    <t>Banggood Order 1</t>
+  </si>
+  <si>
+    <t>Banggood Order 1.pdf</t>
+  </si>
+  <si>
+    <t>120W AC/DC Power Adapter</t>
+  </si>
+  <si>
+    <t>Hobby King Order 3</t>
+  </si>
+  <si>
+    <t>Hobby King Order 3.pdf</t>
+  </si>
+  <si>
+    <t>Higher Voltage, Low KV Motors</t>
+  </si>
+  <si>
+    <t>Digi-Key Order 2</t>
+  </si>
+  <si>
+    <t>Digi-Key Order 1</t>
+  </si>
+  <si>
+    <t>Digi-Key Order 1.pdf</t>
+  </si>
+  <si>
+    <t>5.5x2.5mm Barrel Jacks</t>
   </si>
 </sst>
 </file>
@@ -485,10 +509,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -523,7 +547,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B2" s="5">
         <v>43032</v>
@@ -543,7 +567,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B3" s="5">
         <v>43033</v>
@@ -552,7 +576,7 @@
         <v>7</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E3" s="6">
         <v>48.12</v>
@@ -663,7 +687,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
-        <v>27</v>
+        <v>45</v>
       </c>
       <c r="B9" s="5">
         <v>43084</v>
@@ -672,18 +696,18 @@
         <v>7</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="E9" s="6">
         <v>52.58</v>
       </c>
       <c r="F9" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B10" s="5">
         <v>43084</v>
@@ -692,18 +716,18 @@
         <v>7</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E10" s="6">
         <v>45.22</v>
       </c>
       <c r="F10" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B11" s="5">
         <v>43084</v>
@@ -712,27 +736,82 @@
         <v>7</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E11" s="6">
         <v>147.68</v>
       </c>
       <c r="F11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" s="5">
+        <v>43092</v>
+      </c>
+      <c r="C12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E12" s="6">
+        <v>23.08</v>
+      </c>
+      <c r="F12" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" s="5">
+        <v>43096</v>
+      </c>
+      <c r="C13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E13" s="6">
+        <v>74.790000000000006</v>
+      </c>
+      <c r="F13" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14" s="5">
+        <v>43097</v>
+      </c>
+      <c r="C14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" s="3"/>
+      <c r="F14" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="D16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E16" s="6">
+        <f>SUM(E2:E15)</f>
+        <v>692.99999999999989</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" t="s">
         <v>37</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="D13" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E13" s="6">
-        <f>SUM(E2:E12)</f>
-        <v>595.12999999999988</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" t="s">
-        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -747,8 +826,10 @@
     <hyperlink ref="D9" r:id="rId8" xr:uid="{8125CA67-8455-4019-B4E5-300A48922E7B}"/>
     <hyperlink ref="D10" r:id="rId9" xr:uid="{F602FE1D-63A3-4465-AC92-51C421A80D61}"/>
     <hyperlink ref="D11" r:id="rId10" xr:uid="{A4EDEC9A-1F76-44F4-9AC5-21D8B162BC12}"/>
+    <hyperlink ref="D12" r:id="rId11" xr:uid="{8B5D0249-5887-45D9-9C6E-970A4508ABA1}"/>
+    <hyperlink ref="D13" r:id="rId12" xr:uid="{AACE9272-6814-42DC-B723-7FD6D775BAB6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId11"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId13"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added barrel jack order from Digi-Key to itemized receipts spreadsheet
</commit_message>
<xml_diff>
--- a/Ordered Parts/Itemized Receipts.xlsx
+++ b/Ordered Parts/Itemized Receipts.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18730"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="49">
   <si>
     <t>Description</t>
   </si>
@@ -163,6 +163,9 @@
   </si>
   <si>
     <t>5.5x2.5mm Barrel Jacks</t>
+  </si>
+  <si>
+    <t>Digi-Key Order 2.pdf</t>
   </si>
 </sst>
 </file>
@@ -512,20 +515,20 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.1015625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.47265625" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.47265625" customWidth="1"/>
-    <col min="4" max="4" width="19.20703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.83984375" style="6"/>
-    <col min="6" max="6" width="58.26171875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+    <col min="4" max="4" width="22" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.85546875" style="6"/>
+    <col min="6" max="6" width="58.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -545,7 +548,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>28</v>
       </c>
@@ -565,7 +568,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>29</v>
       </c>
@@ -585,7 +588,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -605,7 +608,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -625,7 +628,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -645,7 +648,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -665,7 +668,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -685,7 +688,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>45</v>
       </c>
@@ -705,7 +708,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>31</v>
       </c>
@@ -725,7 +728,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>36</v>
       </c>
@@ -745,7 +748,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>38</v>
       </c>
@@ -765,7 +768,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>41</v>
       </c>
@@ -785,7 +788,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>44</v>
       </c>
@@ -795,21 +798,26 @@
       <c r="C14" t="s">
         <v>7</v>
       </c>
-      <c r="D14" s="3"/>
+      <c r="D14" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E14" s="6">
+        <v>21.51</v>
+      </c>
       <c r="F14" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D16" s="1" t="s">
         <v>22</v>
       </c>
       <c r="E16" s="6">
         <f>SUM(E2:E15)</f>
-        <v>692.99999999999989</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.55000000000000004">
+        <v>714.50999999999988</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>37</v>
       </c>
@@ -828,8 +836,9 @@
     <hyperlink ref="D11" r:id="rId10" xr:uid="{A4EDEC9A-1F76-44F4-9AC5-21D8B162BC12}"/>
     <hyperlink ref="D12" r:id="rId11" xr:uid="{8B5D0249-5887-45D9-9C6E-970A4508ABA1}"/>
     <hyperlink ref="D13" r:id="rId12" xr:uid="{AACE9272-6814-42DC-B723-7FD6D775BAB6}"/>
+    <hyperlink ref="D14" r:id="rId13" xr:uid="{339F9E84-CD0E-4D83-A0A1-24EBDEF2093A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId13"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId14"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added new Arrow order to itemized receipts spreadsheet
</commit_message>
<xml_diff>
--- a/Ordered Parts/Itemized Receipts.xlsx
+++ b/Ordered Parts/Itemized Receipts.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18730"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="52">
   <si>
     <t>Description</t>
   </si>
@@ -114,12 +114,6 @@
     <t>Hobby King Order 1.pdf</t>
   </si>
   <si>
-    <t>Arrow Order</t>
-  </si>
-  <si>
-    <t>Arrow Order.pdf</t>
-  </si>
-  <si>
     <t>Slip Rings, Power MOSFETs, Rocker Switches</t>
   </si>
   <si>
@@ -166,6 +160,21 @@
   </si>
   <si>
     <t>Digi-Key Order 2.pdf</t>
+  </si>
+  <si>
+    <t>Arrow Order 1.pdf</t>
+  </si>
+  <si>
+    <t>Arrow Order 1</t>
+  </si>
+  <si>
+    <t>Arrow Order 2</t>
+  </si>
+  <si>
+    <t>Arrow Order 2.pdf</t>
+  </si>
+  <si>
+    <t>ATtiny85, Voltage Regulators, Rotary Position Sensors, MOSFETs, SMD Capacitors</t>
   </si>
 </sst>
 </file>
@@ -515,20 +524,20 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+    <col min="1" max="1" width="16.15625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.41796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.41796875" customWidth="1"/>
     <col min="4" max="4" width="22" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.85546875" style="6"/>
-    <col min="6" max="6" width="58.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.83984375" style="6"/>
+    <col min="6" max="6" width="58.26171875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -548,7 +557,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>28</v>
       </c>
@@ -568,7 +577,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>29</v>
       </c>
@@ -588,7 +597,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -608,7 +617,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -628,7 +637,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -648,7 +657,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -668,7 +677,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -688,9 +697,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B9" s="5">
         <v>43084</v>
@@ -699,7 +708,7 @@
         <v>7</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E9" s="6">
         <v>52.58</v>
@@ -708,9 +717,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="B10" s="5">
         <v>43084</v>
@@ -719,18 +728,18 @@
         <v>7</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>32</v>
+        <v>47</v>
       </c>
       <c r="E10" s="6">
         <v>45.22</v>
       </c>
       <c r="F10" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B11" s="5">
         <v>43084</v>
@@ -739,18 +748,18 @@
         <v>7</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E11" s="6">
         <v>147.68</v>
       </c>
       <c r="F11" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B12" s="5">
         <v>43092</v>
@@ -759,18 +768,18 @@
         <v>7</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E12" s="6">
         <v>23.08</v>
       </c>
       <c r="F12" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B13" s="5">
         <v>43096</v>
@@ -779,18 +788,18 @@
         <v>7</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E13" s="6">
         <v>74.790000000000006</v>
       </c>
       <c r="F13" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B14" s="5">
         <v>43097</v>
@@ -799,27 +808,47 @@
         <v>7</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E14" s="6">
         <v>21.51</v>
       </c>
       <c r="F14" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" t="s">
+        <v>49</v>
+      </c>
+      <c r="B15" s="5">
+        <v>43117</v>
+      </c>
+      <c r="C15" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E15" s="6">
+        <v>24.74</v>
+      </c>
+      <c r="F15" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="D16" s="1" t="s">
         <v>22</v>
       </c>
       <c r="E16" s="6">
         <f>SUM(E2:E15)</f>
-        <v>714.50999999999988</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+        <v>739.24999999999989</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -837,8 +866,9 @@
     <hyperlink ref="D12" r:id="rId11" xr:uid="{8B5D0249-5887-45D9-9C6E-970A4508ABA1}"/>
     <hyperlink ref="D13" r:id="rId12" xr:uid="{AACE9272-6814-42DC-B723-7FD6D775BAB6}"/>
     <hyperlink ref="D14" r:id="rId13" xr:uid="{339F9E84-CD0E-4D83-A0A1-24EBDEF2093A}"/>
+    <hyperlink ref="D15" r:id="rId14" xr:uid="{1ADC45DB-9BE6-4D07-8089-248A63109D37}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId14"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId15"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated itemized receipts spreadsheet with latest orders
</commit_message>
<xml_diff>
--- a/Ordered Parts/Itemized Receipts.xlsx
+++ b/Ordered Parts/Itemized Receipts.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19001"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="61">
   <si>
     <t>Description</t>
   </si>
@@ -175,6 +175,33 @@
   </si>
   <si>
     <t>ATtiny85, Voltage Regulators, Rotary Position Sensors, MOSFETs, SMD Capacitors</t>
+  </si>
+  <si>
+    <t>Amazon Order 7</t>
+  </si>
+  <si>
+    <t>Amazon Order 7.pdf</t>
+  </si>
+  <si>
+    <t>M3 screws, M3 standoffs, M3 nuts, M2 screws, M2 nuts, 60W AC/DC Power Adapter</t>
+  </si>
+  <si>
+    <t>Arrow Order 3</t>
+  </si>
+  <si>
+    <t>0.1" PCB headers, receptacles, and crimp contacts</t>
+  </si>
+  <si>
+    <t>OSH Park</t>
+  </si>
+  <si>
+    <t>OSH Park Order.pdf</t>
+  </si>
+  <si>
+    <t>Teensy 3.2</t>
+  </si>
+  <si>
+    <t>Arrow Order 3.pdf</t>
   </si>
 </sst>
 </file>
@@ -521,10 +548,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -838,16 +865,76 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
-      <c r="D16" s="1" t="s">
+      <c r="A16" t="s">
+        <v>52</v>
+      </c>
+      <c r="B16" s="5">
+        <v>43136</v>
+      </c>
+      <c r="C16" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E16" s="6">
+        <v>42.37</v>
+      </c>
+      <c r="F16" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" t="s">
+        <v>55</v>
+      </c>
+      <c r="B17" s="5">
+        <v>43136</v>
+      </c>
+      <c r="C17" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E17" s="6">
+        <v>17.29</v>
+      </c>
+      <c r="F17" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" t="s">
+        <v>57</v>
+      </c>
+      <c r="B18" s="5">
+        <v>43136</v>
+      </c>
+      <c r="C18" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E18" s="6">
+        <v>19</v>
+      </c>
+      <c r="F18" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="D19" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E16" s="6">
-        <f>SUM(E2:E15)</f>
-        <v>739.24999999999989</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" t="s">
+      <c r="E19" s="6">
+        <f>SUM(E2:E18)</f>
+        <v>817.90999999999985</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" t="s">
         <v>35</v>
       </c>
     </row>
@@ -867,8 +954,11 @@
     <hyperlink ref="D13" r:id="rId12" xr:uid="{AACE9272-6814-42DC-B723-7FD6D775BAB6}"/>
     <hyperlink ref="D14" r:id="rId13" xr:uid="{339F9E84-CD0E-4D83-A0A1-24EBDEF2093A}"/>
     <hyperlink ref="D15" r:id="rId14" xr:uid="{1ADC45DB-9BE6-4D07-8089-248A63109D37}"/>
+    <hyperlink ref="D16" r:id="rId15" xr:uid="{C18BBDCF-3AA9-4C7B-8CDB-776A9AD6F102}"/>
+    <hyperlink ref="D18" r:id="rId16" xr:uid="{E923B9F4-7C85-4EB9-B7CE-98BEA9538704}"/>
+    <hyperlink ref="D17" r:id="rId17" xr:uid="{70D213E5-2585-44D5-92CC-E6C60541605E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId15"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId18"/>
 </worksheet>
 </file>
</xml_diff>